<commit_message>
updated component import task
</commit_message>
<xml_diff>
--- a/lib/assets/data_sheets/data_collected.xlsx
+++ b/lib/assets/data_sheets/data_collected.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhimoye/environment/note_titans/lib/assets/data_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD39F70-CDC7-DE4F-B640-3C729C6273C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E827E7-94E9-EB4A-A536-3A3D12D5736C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="3" xr2:uid="{12806AD4-EDD1-E74D-A0E6-8A783616F34F}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="14660" windowHeight="18400" activeTab="4" xr2:uid="{12806AD4-EDD1-E74D-A0E6-8A783616F34F}"/>
   </bookViews>
   <sheets>
     <sheet name="FlashQuests" sheetId="1" r:id="rId1"/>
     <sheet name="MonthlyEvents" sheetId="2" r:id="rId2"/>
     <sheet name="ContentPass" sheetId="3" r:id="rId3"/>
     <sheet name="Components" sheetId="5" r:id="rId4"/>
+    <sheet name="Resources" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="300">
   <si>
     <t>unlock_merchant_level</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1049,6 +1050,142 @@
   </si>
   <si>
     <t>tier</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>resource_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>铁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>木头</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>皮革</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>药草</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>钢</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>硬木</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>布料</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>油</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>珠宝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>以太</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>精华</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>essence</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fabric</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gems</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>herbs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iron</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ironwood</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>leather</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mana</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>oils</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>steel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wood</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Iron</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wood</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Leather</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Herbs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Steel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ironwood</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fabric</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oil</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jewels</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ether</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Essence</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2101,7 +2238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C403D5DA-C305-0848-9697-99072F7D8897}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -2730,4 +2867,152 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99D0BD3D-E0E9-1E49-BDA3-AA829878BD31}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>290</v>
+      </c>
+      <c r="B3" t="s">
+        <v>268</v>
+      </c>
+      <c r="C3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>291</v>
+      </c>
+      <c r="B4" t="s">
+        <v>269</v>
+      </c>
+      <c r="C4" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B5" t="s">
+        <v>270</v>
+      </c>
+      <c r="C5" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>293</v>
+      </c>
+      <c r="B6" t="s">
+        <v>271</v>
+      </c>
+      <c r="C6" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>294</v>
+      </c>
+      <c r="B7" t="s">
+        <v>272</v>
+      </c>
+      <c r="C7" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>295</v>
+      </c>
+      <c r="B8" t="s">
+        <v>273</v>
+      </c>
+      <c r="C8" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>296</v>
+      </c>
+      <c r="B9" t="s">
+        <v>274</v>
+      </c>
+      <c r="C9" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>297</v>
+      </c>
+      <c r="B10" t="s">
+        <v>275</v>
+      </c>
+      <c r="C10" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>298</v>
+      </c>
+      <c r="B11" t="s">
+        <v>276</v>
+      </c>
+      <c r="C11" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>299</v>
+      </c>
+      <c r="B12" t="s">
+        <v>277</v>
+      </c>
+      <c r="C12" t="s">
+        <v>278</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding item type import
</commit_message>
<xml_diff>
--- a/lib/assets/data_sheets/data_collected.xlsx
+++ b/lib/assets/data_sheets/data_collected.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhimoye/environment/note_titans/lib/assets/data_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D281EC6-846E-B34E-8A5F-971FA69F2B84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2FBB8A7-B3C3-F040-B194-DD96BC979013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="14660" windowHeight="17080" firstSheet="2" activeTab="6" xr2:uid="{12806AD4-EDD1-E74D-A0E6-8A783616F34F}"/>
   </bookViews>
@@ -1267,10 +1267,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>subcategory_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>category</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1812,6 +1808,10 @@
   </si>
   <si>
     <t>Runestone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type_id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3706,7 +3706,7 @@
         <v>310</v>
       </c>
       <c r="B5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C5" t="s">
         <v>304</v>
@@ -3745,7 +3745,7 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3762,27 +3762,27 @@
         <v>65</v>
       </c>
       <c r="C1" t="s">
+        <v>455</v>
+      </c>
+      <c r="D1" t="s">
+        <v>428</v>
+      </c>
+      <c r="E1" t="s">
         <v>319</v>
-      </c>
-      <c r="D1" t="s">
-        <v>429</v>
-      </c>
-      <c r="E1" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B2" t="s">
         <v>323</v>
       </c>
-      <c r="B2" t="s">
-        <v>324</v>
-      </c>
       <c r="C2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E2" t="s">
         <v>301</v>
@@ -3790,16 +3790,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E3" t="s">
         <v>302</v>
@@ -3807,16 +3807,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E4" t="s">
         <v>302</v>
@@ -3824,16 +3824,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E5" t="s">
         <v>302</v>
@@ -3841,16 +3841,16 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D6" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E6" t="s">
         <v>301</v>
@@ -3858,16 +3858,16 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D7" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E7" t="s">
         <v>306</v>
@@ -3875,16 +3875,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D8" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E8" t="s">
         <v>303</v>
@@ -3892,16 +3892,16 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C9" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D9" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E9" t="s">
         <v>306</v>
@@ -3909,16 +3909,16 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B10" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C10" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D10" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E10" t="s">
         <v>303</v>
@@ -3926,16 +3926,16 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B11" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C11" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D11" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E11" t="s">
         <v>301</v>
@@ -3943,16 +3943,16 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B12" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C12" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E12" t="s">
         <v>306</v>
@@ -3960,16 +3960,16 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C13" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D13" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E13" t="s">
         <v>306</v>
@@ -3977,16 +3977,16 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B14" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D14" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E14" t="s">
         <v>301</v>
@@ -3994,16 +3994,16 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
+        <v>348</v>
+      </c>
+      <c r="B15" t="s">
         <v>349</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>350</v>
       </c>
-      <c r="C15" t="s">
-        <v>351</v>
-      </c>
       <c r="D15" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E15" t="s">
         <v>304</v>
@@ -4011,16 +4011,16 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B16" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C16" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D16" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E16" t="s">
         <v>301</v>
@@ -4028,16 +4028,16 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B17" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C17" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D17" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E17" t="s">
         <v>303</v>
@@ -4045,16 +4045,16 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B18" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C18" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D18" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E18" t="s">
         <v>306</v>
@@ -4062,16 +4062,16 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B19" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C19" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E19" t="s">
         <v>303</v>
@@ -4079,16 +4079,16 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B20" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C20" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D20" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E20" t="s">
         <v>303</v>
@@ -4096,16 +4096,16 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B21" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C21" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D21" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E21" t="s">
         <v>301</v>
@@ -4113,16 +4113,16 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B22" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C22" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D22" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E22" t="s">
         <v>306</v>
@@ -4130,16 +4130,16 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B23" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C23" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D23" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E23" t="s">
         <v>306</v>
@@ -4147,16 +4147,16 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B24" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C24" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D24" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E24" t="s">
         <v>301</v>
@@ -4164,13 +4164,13 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B25" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C25" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D25" t="s">
         <v>22</v>
@@ -4181,16 +4181,16 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B26" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C26" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D26" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E26" t="s">
         <v>301</v>
@@ -4198,16 +4198,16 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B27" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C27" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D27" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E27" t="s">
         <v>301</v>
@@ -4215,16 +4215,16 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B28" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C28" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D28" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E28" t="s">
         <v>303</v>
@@ -4232,13 +4232,13 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B29" t="s">
         <v>318</v>
       </c>
       <c r="C29" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D29" t="s">
         <v>25</v>
@@ -4249,16 +4249,16 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B30" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C30" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D30" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E30" t="s">
         <v>301</v>
@@ -4266,16 +4266,16 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B31" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C31" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D31" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E31" t="s">
         <v>301</v>
@@ -4283,16 +4283,16 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B32" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C32" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D32" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E32" t="s">
         <v>303</v>
@@ -4300,16 +4300,16 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B33" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C33" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D33" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E33" t="s">
         <v>306</v>
@@ -4317,16 +4317,16 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B34" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C34" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D34" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E34" t="s">
         <v>304</v>
@@ -4334,16 +4334,16 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B35" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C35" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D35" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E35" t="s">
         <v>306</v>
@@ -4351,16 +4351,16 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B36" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C36" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D36" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E36" t="s">
         <v>306</v>
@@ -4368,16 +4368,16 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B37" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C37" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D37" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E37" t="s">
         <v>306</v>

</xml_diff>

<commit_message>
add workers and blueprint unlock type import
</commit_message>
<xml_diff>
--- a/lib/assets/data_sheets/data_collected.xlsx
+++ b/lib/assets/data_sheets/data_collected.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhimoye/environment/note_titans/lib/assets/data_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3A1559-66CE-DB42-AD04-ED52B065D544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1865BF-3ED2-1246-9957-D0EA22F1EFBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17080" firstSheet="2" activeTab="8" xr2:uid="{12806AD4-EDD1-E74D-A0E6-8A783616F34F}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16780" firstSheet="2" activeTab="10" xr2:uid="{12806AD4-EDD1-E74D-A0E6-8A783616F34F}"/>
   </bookViews>
   <sheets>
     <sheet name="FlashQuests" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,8 @@
     <sheet name="ContentPass" sheetId="3" r:id="rId7"/>
     <sheet name="Blueprints" sheetId="10" r:id="rId8"/>
     <sheet name="Quality" sheetId="11" r:id="rId9"/>
+    <sheet name="BlueprintType" sheetId="12" r:id="rId10"/>
+    <sheet name="Worker" sheetId="13" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3801" uniqueCount="3737">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3887" uniqueCount="3821">
   <si>
     <t>unlock_merchant_level</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -11677,6 +11679,326 @@
   </si>
   <si>
     <t>Superior</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>artifact</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>blue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lcog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>premium</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>description_en</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>description_zh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>神器图纸，从神器宝箱中开出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>基础图纸，通过游戏进程免费获得</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>宝箱图纸，通过冒险获得</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高级图纸，通过购买礼包解锁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Artifact blueprints, unlock from Artifact Chests</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Basic blueprints, unlock from game process</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chest blueprints, unlock from Quest Chests</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lost City of Gold blueprints, unlock from LCoG Events or Chests.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>黄金城图纸，通过黄金城活动奖励或宝箱获得</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Premium blueprints, unlock by purchasing in-game pack or offers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>worker_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Blacksmith</t>
+  </si>
+  <si>
+    <t>Tailor</t>
+  </si>
+  <si>
+    <t>Carpenter</t>
+  </si>
+  <si>
+    <t>Herbalist</t>
+  </si>
+  <si>
+    <t>Wizard</t>
+  </si>
+  <si>
+    <t>Jeweler</t>
+  </si>
+  <si>
+    <t>Priestess</t>
+  </si>
+  <si>
+    <t>Master</t>
+  </si>
+  <si>
+    <t>Scholar</t>
+  </si>
+  <si>
+    <t>Engineer</t>
+  </si>
+  <si>
+    <t>Sun Dragon</t>
+  </si>
+  <si>
+    <t>Moon Dragon</t>
+  </si>
+  <si>
+    <t>Summoner</t>
+  </si>
+  <si>
+    <t>Cook</t>
+  </si>
+  <si>
+    <t>Baker</t>
+  </si>
+  <si>
+    <t>Bard</t>
+  </si>
+  <si>
+    <t>华莱士</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>茱莉亚</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>艾伦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>玛丽贝尔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>格里玛尔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>卡特琳娜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>弗雷娅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>伊芙琳</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>罗克珊</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>桑达拉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>穆达拉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>尤兰达</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图图·马诺</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>派柯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>约翰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>academy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baker</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>blacksmith</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>carpenter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cook</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>elven</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>engineer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>herbalist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jeweler</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>master</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>moondragon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>priest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sundragon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tailor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wizard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>profession_en</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>profession_zh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>希欧多尔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大师</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阳龙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>草药师</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>女魔术师</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>铁匠</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>魔法师</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>珠宝匠</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>木匠</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工程师</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>裁缝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>厨师</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学士</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>月龙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>吟游诗人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤师</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>烘焙师</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -12413,6 +12735,345 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74E3B92D-19C2-8D4C-A20D-A7DE542210AB}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="60.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>431</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3742</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3743</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>3737</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3748</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3744</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>3738</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3749</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3745</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>3739</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3750</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3746</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>3740</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3751</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3752</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>3741</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3753</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3747</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1432A11-034F-7949-A987-7734190589CB}">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>3802</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3754</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3803</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>3755</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3771</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3789</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3809</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>3756</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3772</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3800</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3814</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>3757</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3773</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3790</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3812</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2" t="s">
+        <v>3758</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3774</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3794</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3807</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>3759</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3775</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3801</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3810</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>3760</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3776</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3795</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3811</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>3761</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3777</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3798</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3808</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2" t="s">
+        <v>3762</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3804</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3796</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3805</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2" t="s">
+        <v>3763</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3778</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3786</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3816</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="2" t="s">
+        <v>3764</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3779</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3793</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3813</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="2" t="s">
+        <v>3765</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3780</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3799</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3806</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="2" t="s">
+        <v>3766</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3781</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3797</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3817</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="2" t="s">
+        <v>3767</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3782</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3792</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3819</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="2" t="s">
+        <v>3768</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3783</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3791</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3815</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="2" t="s">
+        <v>3769</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3784</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3787</v>
+      </c>
+      <c r="D16" t="s">
+        <v>3820</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="2" t="s">
+        <v>3770</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3785</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3788</v>
+      </c>
+      <c r="D17" t="s">
+        <v>3818</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CE4324-2568-3749-AED0-5A678396A05D}">
   <dimension ref="A1:E5"/>
@@ -26335,8 +26996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3E789D7-1DD7-A44F-A51F-B2B30843194C}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
add atlab item images
</commit_message>
<xml_diff>
--- a/lib/assets/data_sheets/data_collected.xlsx
+++ b/lib/assets/data_sheets/data_collected.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhimoye/environment/note_titans/lib/assets/data_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22C643C-DF71-8B40-B585-4B0EE8A7FAD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F9436ED-60FD-C740-8164-B5951C4B6C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16780" firstSheet="2" activeTab="7" xr2:uid="{12806AD4-EDD1-E74D-A0E6-8A783616F34F}"/>
   </bookViews>
@@ -12449,10 +12449,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>darknightboots</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>summerbodshoes</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -12538,6 +12534,10 @@
   </si>
   <si>
     <t>behemoth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>darkknightboots</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -15535,8 +15535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E80B504A-1FA4-7246-8FE4-C307A80553BD}">
   <dimension ref="A1:C1137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1121" zoomScale="208" zoomScaleNormal="208" workbookViewId="0">
-      <selection activeCell="C1132" sqref="C1132"/>
+    <sheetView tabSelected="1" topLeftCell="A1106" zoomScale="208" zoomScaleNormal="208" workbookViewId="0">
+      <selection activeCell="C1115" sqref="C1115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -27798,7 +27798,7 @@
         <v>3896</v>
       </c>
       <c r="C1114" s="4" t="s">
-        <v>3945</v>
+        <v>3967</v>
       </c>
     </row>
     <row r="1115" spans="1:3">
@@ -27820,7 +27820,7 @@
         <v>3898</v>
       </c>
       <c r="C1116" s="4" t="s">
-        <v>3946</v>
+        <v>3945</v>
       </c>
     </row>
     <row r="1117" spans="1:3">
@@ -27831,7 +27831,7 @@
         <v>3899</v>
       </c>
       <c r="C1117" s="4" t="s">
-        <v>3947</v>
+        <v>3946</v>
       </c>
     </row>
     <row r="1118" spans="1:3">
@@ -27842,7 +27842,7 @@
         <v>3900</v>
       </c>
       <c r="C1118" s="4" t="s">
-        <v>3948</v>
+        <v>3947</v>
       </c>
     </row>
     <row r="1119" spans="1:3">
@@ -27853,7 +27853,7 @@
         <v>3901</v>
       </c>
       <c r="C1119" s="4" t="s">
-        <v>3949</v>
+        <v>3948</v>
       </c>
     </row>
     <row r="1120" spans="1:3">
@@ -27864,7 +27864,7 @@
         <v>3902</v>
       </c>
       <c r="C1120" s="4" t="s">
-        <v>3950</v>
+        <v>3949</v>
       </c>
     </row>
     <row r="1121" spans="1:3">
@@ -27875,7 +27875,7 @@
         <v>3903</v>
       </c>
       <c r="C1121" s="4" t="s">
-        <v>3951</v>
+        <v>3950</v>
       </c>
     </row>
     <row r="1122" spans="1:3">
@@ -27886,7 +27886,7 @@
         <v>3904</v>
       </c>
       <c r="C1122" s="4" t="s">
-        <v>3952</v>
+        <v>3951</v>
       </c>
     </row>
     <row r="1123" spans="1:3">
@@ -27897,7 +27897,7 @@
         <v>3905</v>
       </c>
       <c r="C1123" s="4" t="s">
-        <v>3953</v>
+        <v>3952</v>
       </c>
     </row>
     <row r="1124" spans="1:3">
@@ -27908,7 +27908,7 @@
         <v>3906</v>
       </c>
       <c r="C1124" s="4" t="s">
-        <v>3954</v>
+        <v>3953</v>
       </c>
     </row>
     <row r="1125" spans="1:3">
@@ -27919,7 +27919,7 @@
         <v>3907</v>
       </c>
       <c r="C1125" s="4" t="s">
-        <v>3958</v>
+        <v>3957</v>
       </c>
     </row>
     <row r="1126" spans="1:3">
@@ -27930,7 +27930,7 @@
         <v>3908</v>
       </c>
       <c r="C1126" s="4" t="s">
-        <v>3960</v>
+        <v>3959</v>
       </c>
     </row>
     <row r="1127" spans="1:3">
@@ -27941,7 +27941,7 @@
         <v>3909</v>
       </c>
       <c r="C1127" s="4" t="s">
-        <v>3955</v>
+        <v>3954</v>
       </c>
     </row>
     <row r="1128" spans="1:3">
@@ -27952,7 +27952,7 @@
         <v>3910</v>
       </c>
       <c r="C1128" s="4" t="s">
-        <v>3957</v>
+        <v>3956</v>
       </c>
     </row>
     <row r="1129" spans="1:3">
@@ -27963,7 +27963,7 @@
         <v>3911</v>
       </c>
       <c r="C1129" s="4" t="s">
-        <v>3959</v>
+        <v>3958</v>
       </c>
     </row>
     <row r="1130" spans="1:3">
@@ -27974,7 +27974,7 @@
         <v>3912</v>
       </c>
       <c r="C1130" s="4" t="s">
-        <v>3956</v>
+        <v>3955</v>
       </c>
     </row>
     <row r="1131" spans="1:3">
@@ -27985,7 +27985,7 @@
         <v>3913</v>
       </c>
       <c r="C1131" s="4" t="s">
-        <v>3962</v>
+        <v>3961</v>
       </c>
     </row>
     <row r="1132" spans="1:3">
@@ -27996,7 +27996,7 @@
         <v>3914</v>
       </c>
       <c r="C1132" s="4" t="s">
-        <v>3967</v>
+        <v>3966</v>
       </c>
     </row>
     <row r="1133" spans="1:3">
@@ -28007,7 +28007,7 @@
         <v>3915</v>
       </c>
       <c r="C1133" s="4" t="s">
-        <v>3965</v>
+        <v>3964</v>
       </c>
     </row>
     <row r="1134" spans="1:3">
@@ -28018,7 +28018,7 @@
         <v>3916</v>
       </c>
       <c r="C1134" s="4" t="s">
-        <v>3961</v>
+        <v>3960</v>
       </c>
     </row>
     <row r="1135" spans="1:3">
@@ -28029,7 +28029,7 @@
         <v>3917</v>
       </c>
       <c r="C1135" s="4" t="s">
-        <v>3964</v>
+        <v>3963</v>
       </c>
     </row>
     <row r="1136" spans="1:3">
@@ -28040,7 +28040,7 @@
         <v>3918</v>
       </c>
       <c r="C1136" s="4" t="s">
-        <v>3963</v>
+        <v>3962</v>
       </c>
     </row>
     <row r="1137" spans="1:3">
@@ -28051,7 +28051,7 @@
         <v>3919</v>
       </c>
       <c r="C1137" s="4" t="s">
-        <v>3966</v>
+        <v>3965</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add humanize gem for number word conversion, add basic blueprint_card css style
</commit_message>
<xml_diff>
--- a/lib/assets/data_sheets/data_collected.xlsx
+++ b/lib/assets/data_sheets/data_collected.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhimoye/environment/note_titans/lib/assets/data_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F9436ED-60FD-C740-8164-B5951C4B6C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED10F4C3-96C1-5C4B-BFE8-861DD1C42E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16780" firstSheet="2" activeTab="7" xr2:uid="{12806AD4-EDD1-E74D-A0E6-8A783616F34F}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16780" firstSheet="2" activeTab="5" xr2:uid="{12806AD4-EDD1-E74D-A0E6-8A783616F34F}"/>
   </bookViews>
   <sheets>
     <sheet name="FlashQuests" sheetId="1" r:id="rId1"/>
@@ -14611,7 +14611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EC91502-E205-114E-9B1A-0C577B332A42}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView zoomScale="112" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -15535,7 +15535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E80B504A-1FA4-7246-8FE4-C307A80553BD}">
   <dimension ref="A1:C1137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1106" zoomScale="208" zoomScaleNormal="208" workbookViewId="0">
+    <sheetView topLeftCell="A1106" zoomScale="208" zoomScaleNormal="208" workbookViewId="0">
       <selection activeCell="C1115" sqref="C1115"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
modify models, preload database for blueprint index page, add global imgs into helper.rb
</commit_message>
<xml_diff>
--- a/lib/assets/data_sheets/data_collected.xlsx
+++ b/lib/assets/data_sheets/data_collected.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhimoye/environment/note_titans/lib/assets/data_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED10F4C3-96C1-5C4B-BFE8-861DD1C42E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727B8544-5294-7E46-8D61-8E2A5B08E840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16780" firstSheet="2" activeTab="5" xr2:uid="{12806AD4-EDD1-E74D-A0E6-8A783616F34F}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="14660" windowHeight="18400" firstSheet="2" activeTab="6" xr2:uid="{12806AD4-EDD1-E74D-A0E6-8A783616F34F}"/>
   </bookViews>
   <sheets>
     <sheet name="FlashQuests" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,12 @@
     <sheet name="Resources" sheetId="6" r:id="rId4"/>
     <sheet name="Category" sheetId="7" r:id="rId5"/>
     <sheet name="Type" sheetId="8" r:id="rId6"/>
-    <sheet name="ContentPass" sheetId="3" r:id="rId7"/>
-    <sheet name="Blueprints" sheetId="10" r:id="rId8"/>
-    <sheet name="Quality" sheetId="11" r:id="rId9"/>
-    <sheet name="BlueprintType" sheetId="12" r:id="rId10"/>
-    <sheet name="Worker" sheetId="13" r:id="rId11"/>
+    <sheet name="Affinity" sheetId="14" r:id="rId7"/>
+    <sheet name="ContentPass" sheetId="3" r:id="rId8"/>
+    <sheet name="Blueprints" sheetId="10" r:id="rId9"/>
+    <sheet name="Quality" sheetId="11" r:id="rId10"/>
+    <sheet name="BlueprintType" sheetId="12" r:id="rId11"/>
+    <sheet name="Worker" sheetId="13" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4034" uniqueCount="3968">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4175" uniqueCount="4009">
   <si>
     <t>unlock_merchant_level</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -12538,6 +12539,170 @@
   </si>
   <si>
     <t>darkknightboots</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enchantment_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>affinity_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fire</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>water</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>air</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>earth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>light</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dark</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gold</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>armadillo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bear</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>carbuncle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chimera</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>crab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dinosaur</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enchantment_id=blueprint_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dragon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eagle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>freshspirit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hippo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hydra</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kraken</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lizard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>luxuriousspirit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mammoth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>opulentspirit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>owl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ox</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>phoenix</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rabbitspirit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rhino</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>santa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shark</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tarrasque</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tiger</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>turtle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>viper</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>walrus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wolf</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -12545,7 +12710,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -12621,6 +12786,16 @@
       <name val="Arial Unicode MS"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF20124D"/>
+      <name val="Droid Sans"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF783F04"/>
+      <name val="Droid Sans"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -12644,7 +12819,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -12672,6 +12847,12 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -13283,6 +13464,88 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3E789D7-1DD7-A44F-A51F-B2B30843194C}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>3721</v>
+      </c>
+      <c r="B1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>3722</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3735</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3730</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>3725</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3736</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3731</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>3724</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3727</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3732</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>3723</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3728</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3733</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>3726</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3729</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3734</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74E3B92D-19C2-8D4C-A20D-A7DE542210AB}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -13367,7 +13630,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1432A11-034F-7949-A987-7734190589CB}">
   <dimension ref="A1:D17"/>
   <sheetViews>
@@ -14611,7 +14874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EC91502-E205-114E-9B1A-0C577B332A42}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
+    <sheetView zoomScale="112" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -15257,6 +15520,591 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9284AFDF-38E2-6C44-96DE-41340047FC8F}">
+  <dimension ref="A1:C71"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>3968</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3969</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3984</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>3556</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3970</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>3559</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3970</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2" t="s">
+        <v>3562</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3970</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2" t="s">
+        <v>3565</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3970</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="2" t="s">
+        <v>3859</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3970</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="2" t="s">
+        <v>3568</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3971</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="2" t="s">
+        <v>3571</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3971</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="2" t="s">
+        <v>3574</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3971</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="2" t="s">
+        <v>3577</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3971</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="2" t="s">
+        <v>3860</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3971</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="2" t="s">
+        <v>3580</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3972</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="2" t="s">
+        <v>3583</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3972</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="2" t="s">
+        <v>3586</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3972</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="2" t="s">
+        <v>3589</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3972</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="2" t="s">
+        <v>3861</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3972</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="2" t="s">
+        <v>3592</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3973</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="2" t="s">
+        <v>3595</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3973</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="2" t="s">
+        <v>3598</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3973</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="2" t="s">
+        <v>3601</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3973</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="2" t="s">
+        <v>3862</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3973</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="2" t="s">
+        <v>3604</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3974</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="2" t="s">
+        <v>3607</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3974</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="2" t="s">
+        <v>3610</v>
+      </c>
+      <c r="B24" t="s">
+        <v>3974</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="2" t="s">
+        <v>3613</v>
+      </c>
+      <c r="B25" t="s">
+        <v>3974</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="2" t="s">
+        <v>3863</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3974</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="2" t="s">
+        <v>3616</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3975</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="2" t="s">
+        <v>3619</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3975</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="2" t="s">
+        <v>3622</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3975</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="2" t="s">
+        <v>3625</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3975</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="2" t="s">
+        <v>3864</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3975</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="11" t="s">
+        <v>3628</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3976</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="11" t="s">
+        <v>3631</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3976</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="2" t="s">
+        <v>3634</v>
+      </c>
+      <c r="B34" t="s">
+        <v>4005</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="2" t="s">
+        <v>3637</v>
+      </c>
+      <c r="B35" t="s">
+        <v>4008</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="2" t="s">
+        <v>3640</v>
+      </c>
+      <c r="B36" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="2" t="s">
+        <v>3643</v>
+      </c>
+      <c r="B37" t="s">
+        <v>3986</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="2" t="s">
+        <v>3646</v>
+      </c>
+      <c r="B38" t="s">
+        <v>4006</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="2" t="s">
+        <v>3649</v>
+      </c>
+      <c r="B39" t="s">
+        <v>3980</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="2" t="s">
+        <v>3652</v>
+      </c>
+      <c r="B40" t="s">
+        <v>3999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="2" t="s">
+        <v>3865</v>
+      </c>
+      <c r="B41" t="s">
+        <v>3961</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="11" t="s">
+        <v>3655</v>
+      </c>
+      <c r="B42" t="s">
+        <v>3993</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="2" t="s">
+        <v>3658</v>
+      </c>
+      <c r="B43" t="s">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="2" t="s">
+        <v>3661</v>
+      </c>
+      <c r="B44" t="s">
+        <v>3996</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="2" t="s">
+        <v>3664</v>
+      </c>
+      <c r="B45" t="s">
+        <v>3977</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="2" t="s">
+        <v>3667</v>
+      </c>
+      <c r="B46" t="s">
+        <v>3992</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="2" t="s">
+        <v>3670</v>
+      </c>
+      <c r="B47" t="s">
+        <v>3982</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="2" t="s">
+        <v>3673</v>
+      </c>
+      <c r="B48" t="s">
+        <v>3988</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="2" t="s">
+        <v>3676</v>
+      </c>
+      <c r="B49" t="s">
+        <v>4002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="2" t="s">
+        <v>3679</v>
+      </c>
+      <c r="B50" t="s">
+        <v>4007</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="2" t="s">
+        <v>3682</v>
+      </c>
+      <c r="B51" t="s">
+        <v>3991</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="2" t="s">
+        <v>3685</v>
+      </c>
+      <c r="B52" t="s">
+        <v>3978</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="2" t="s">
+        <v>3688</v>
+      </c>
+      <c r="B53" t="s">
+        <v>3994</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="2" t="s">
+        <v>3691</v>
+      </c>
+      <c r="B54" t="s">
+        <v>3983</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="2" t="s">
+        <v>3694</v>
+      </c>
+      <c r="B55" t="s">
+        <v>4004</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="11" t="s">
+        <v>3697</v>
+      </c>
+      <c r="B56" t="s">
+        <v>3995</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="2" t="s">
+        <v>3700</v>
+      </c>
+      <c r="B57" t="s">
+        <v>3998</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="2" t="s">
+        <v>3703</v>
+      </c>
+      <c r="B58" t="s">
+        <v>3989</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="2" t="s">
+        <v>3706</v>
+      </c>
+      <c r="B59" t="s">
+        <v>4003</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="2" t="s">
+        <v>3709</v>
+      </c>
+      <c r="B60" t="s">
+        <v>3979</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="2" t="s">
+        <v>3712</v>
+      </c>
+      <c r="B61" t="s">
+        <v>3981</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="2" t="s">
+        <v>3715</v>
+      </c>
+      <c r="B62" t="s">
+        <v>3990</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="12" t="s">
+        <v>3718</v>
+      </c>
+      <c r="B63" t="s">
+        <v>4001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="2" t="s">
+        <v>3866</v>
+      </c>
+      <c r="B64" t="s">
+        <v>3966</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="2" t="s">
+        <v>3867</v>
+      </c>
+      <c r="B65" t="s">
+        <v>3964</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="2" t="s">
+        <v>3868</v>
+      </c>
+      <c r="B66" t="s">
+        <v>3960</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="2" t="s">
+        <v>3869</v>
+      </c>
+      <c r="B67" t="s">
+        <v>3963</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="2" t="s">
+        <v>3870</v>
+      </c>
+      <c r="B68" t="s">
+        <v>3962</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="2" t="s">
+        <v>3871</v>
+      </c>
+      <c r="B69" t="s">
+        <v>3965</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="B70" t="s">
+        <v>3985</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="B71" t="s">
+        <v>3987</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA03D614-9D25-014E-BEA0-F56DD3E0919C}">
   <dimension ref="A1:F13"/>
   <sheetViews>
@@ -15531,7 +16379,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E80B504A-1FA4-7246-8FE4-C307A80553BD}">
   <dimension ref="A1:C1137"/>
   <sheetViews>
@@ -28058,86 +28906,4 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3E789D7-1DD7-A44F-A51F-B2B30843194C}">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>3721</v>
-      </c>
-      <c r="B1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>3722</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3735</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3730</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>3725</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3736</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3731</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>3724</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3727</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3732</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>3723</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3728</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3733</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>3726</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3729</v>
-      </c>
-      <c r="C6" t="s">
-        <v>3734</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add olympic blueprints, remove unnecessary translations in locale ymls, add database:check_update task, implemented basic category filter in views
</commit_message>
<xml_diff>
--- a/lib/assets/data_sheets/data_collected.xlsx
+++ b/lib/assets/data_sheets/data_collected.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhimoye/environment/note_titans/lib/assets/data_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727B8544-5294-7E46-8D61-8E2A5B08E840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D0DD6F-8D44-AA4C-957F-89D390C66EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="14660" windowHeight="18400" firstSheet="2" activeTab="6" xr2:uid="{12806AD4-EDD1-E74D-A0E6-8A783616F34F}"/>
+    <workbookView xWindow="1300" yWindow="740" windowWidth="14660" windowHeight="17080" firstSheet="4" activeTab="8" xr2:uid="{12806AD4-EDD1-E74D-A0E6-8A783616F34F}"/>
   </bookViews>
   <sheets>
     <sheet name="FlashQuests" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4175" uniqueCount="4009">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4184" uniqueCount="4018">
   <si>
     <t>unlock_merchant_level</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -12703,6 +12703,42 @@
   </si>
   <si>
     <t>wolf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>olympicspear</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>奥林匹亚标枪</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Olympian Javelin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Aura of Victory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>金牌</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>胜利光环</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>olympicamulet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>olympicaura</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gold Medal</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -14778,7 +14814,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -14800,13 +14836,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="B2" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="C2" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -14833,35 +14869,35 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B5" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="C5" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B6" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="C6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -14874,8 +14910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EC91502-E205-114E-9B1A-0C577B332A42}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView zoomScale="112" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A8" zoomScale="112" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -14903,101 +14939,101 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>298</v>
+        <v>405</v>
       </c>
       <c r="B2" t="s">
-        <v>299</v>
+        <v>367</v>
       </c>
       <c r="C2" t="s">
-        <v>297</v>
+        <v>366</v>
       </c>
       <c r="D2" t="s">
-        <v>370</v>
+        <v>402</v>
       </c>
       <c r="E2" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>384</v>
+        <v>406</v>
       </c>
       <c r="B3" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
       <c r="C3" t="s">
-        <v>300</v>
+        <v>308</v>
       </c>
       <c r="D3" t="s">
-        <v>384</v>
+        <v>372</v>
       </c>
       <c r="E3" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>375</v>
+        <v>407</v>
       </c>
       <c r="B4" t="s">
-        <v>304</v>
+        <v>321</v>
       </c>
       <c r="C4" t="s">
-        <v>301</v>
+        <v>320</v>
       </c>
       <c r="D4" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="E4" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>389</v>
+        <v>408</v>
       </c>
       <c r="B5" t="s">
-        <v>305</v>
+        <v>342</v>
       </c>
       <c r="C5" t="s">
-        <v>302</v>
+        <v>341</v>
       </c>
       <c r="D5" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="E5" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>427</v>
+        <v>409</v>
       </c>
       <c r="B6" t="s">
-        <v>307</v>
+        <v>361</v>
       </c>
       <c r="C6" t="s">
-        <v>306</v>
+        <v>360</v>
       </c>
       <c r="D6" t="s">
-        <v>371</v>
+        <v>398</v>
       </c>
       <c r="E6" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="B7" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="C7" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="D7" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E7" t="s">
         <v>282</v>
@@ -15005,33 +15041,33 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>385</v>
+        <v>412</v>
       </c>
       <c r="B8" t="s">
-        <v>311</v>
+        <v>369</v>
       </c>
       <c r="C8" t="s">
-        <v>310</v>
+        <v>368</v>
       </c>
       <c r="D8" t="s">
-        <v>385</v>
+        <v>403</v>
       </c>
       <c r="E8" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B9" t="s">
-        <v>313</v>
+        <v>365</v>
       </c>
       <c r="C9" t="s">
-        <v>312</v>
+        <v>364</v>
       </c>
       <c r="D9" t="s">
-        <v>373</v>
+        <v>401</v>
       </c>
       <c r="E9" t="s">
         <v>282</v>
@@ -15039,50 +15075,50 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>382</v>
+        <v>414</v>
       </c>
       <c r="B10" t="s">
-        <v>315</v>
+        <v>332</v>
       </c>
       <c r="C10" t="s">
-        <v>314</v>
+        <v>331</v>
       </c>
       <c r="D10" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="E10" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
       <c r="B11" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="C11" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D11" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="E11" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="B12" t="s">
-        <v>319</v>
+        <v>340</v>
       </c>
       <c r="C12" t="s">
-        <v>318</v>
+        <v>339</v>
       </c>
       <c r="D12" t="s">
-        <v>376</v>
+        <v>388</v>
       </c>
       <c r="E12" t="s">
         <v>282</v>
@@ -15090,84 +15126,84 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>407</v>
+        <v>384</v>
       </c>
       <c r="B13" t="s">
-        <v>321</v>
+        <v>303</v>
       </c>
       <c r="C13" t="s">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="D13" t="s">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="E13" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>426</v>
+        <v>389</v>
       </c>
       <c r="B14" t="s">
-        <v>323</v>
+        <v>305</v>
       </c>
       <c r="C14" t="s">
-        <v>322</v>
+        <v>302</v>
       </c>
       <c r="D14" t="s">
-        <v>378</v>
+        <v>389</v>
       </c>
       <c r="E14" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>324</v>
+        <v>375</v>
       </c>
       <c r="B15" t="s">
-        <v>325</v>
+        <v>304</v>
       </c>
       <c r="C15" t="s">
-        <v>326</v>
+        <v>301</v>
       </c>
       <c r="D15" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="E15" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="B16" t="s">
-        <v>328</v>
+        <v>336</v>
       </c>
       <c r="C16" t="s">
-        <v>327</v>
+        <v>335</v>
       </c>
       <c r="D16" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="E16" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>381</v>
+        <v>419</v>
       </c>
       <c r="B17" t="s">
-        <v>330</v>
+        <v>352</v>
       </c>
       <c r="C17" t="s">
-        <v>329</v>
+        <v>351</v>
       </c>
       <c r="D17" t="s">
-        <v>381</v>
+        <v>396</v>
       </c>
       <c r="E17" t="s">
         <v>279</v>
@@ -15175,33 +15211,33 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>414</v>
+        <v>420</v>
       </c>
       <c r="B18" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="C18" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D18" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="E18" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>420</v>
+        <v>381</v>
       </c>
       <c r="B19" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C19" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D19" t="s">
-        <v>392</v>
+        <v>381</v>
       </c>
       <c r="E19" t="s">
         <v>279</v>
@@ -15209,16 +15245,16 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>418</v>
+        <v>382</v>
       </c>
       <c r="B20" t="s">
-        <v>336</v>
+        <v>315</v>
       </c>
       <c r="C20" t="s">
-        <v>335</v>
+        <v>314</v>
       </c>
       <c r="D20" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="E20" t="s">
         <v>279</v>
@@ -15226,67 +15262,67 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B21" t="s">
-        <v>338</v>
+        <v>311</v>
       </c>
       <c r="C21" t="s">
-        <v>337</v>
+        <v>310</v>
       </c>
       <c r="D21" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E21" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>415</v>
+        <v>390</v>
       </c>
       <c r="B22" t="s">
-        <v>340</v>
+        <v>359</v>
       </c>
       <c r="C22" t="s">
-        <v>339</v>
+        <v>358</v>
       </c>
       <c r="D22" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="E22" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>408</v>
+        <v>387</v>
       </c>
       <c r="B23" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="C23" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D23" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="E23" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>425</v>
+        <v>416</v>
       </c>
       <c r="B24" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="C24" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="D24" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="E24" t="s">
         <v>277</v>
@@ -15294,33 +15330,33 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>429</v>
+        <v>417</v>
       </c>
       <c r="B25" t="s">
-        <v>346</v>
+        <v>355</v>
       </c>
       <c r="C25" t="s">
-        <v>345</v>
+        <v>354</v>
       </c>
       <c r="D25" t="s">
-        <v>22</v>
+        <v>399</v>
       </c>
       <c r="E25" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="B26" t="s">
-        <v>348</v>
+        <v>357</v>
       </c>
       <c r="C26" t="s">
-        <v>347</v>
+        <v>356</v>
       </c>
       <c r="D26" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="E26" t="s">
         <v>277</v>
@@ -15345,50 +15381,50 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>419</v>
+        <v>298</v>
       </c>
       <c r="B28" t="s">
-        <v>352</v>
+        <v>299</v>
       </c>
       <c r="C28" t="s">
-        <v>351</v>
+        <v>297</v>
       </c>
       <c r="D28" t="s">
-        <v>396</v>
+        <v>370</v>
       </c>
       <c r="E28" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="B29" t="s">
-        <v>294</v>
+        <v>317</v>
       </c>
       <c r="C29" t="s">
-        <v>353</v>
+        <v>316</v>
       </c>
       <c r="D29" t="s">
-        <v>25</v>
+        <v>374</v>
       </c>
       <c r="E29" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>417</v>
+        <v>424</v>
       </c>
       <c r="B30" t="s">
-        <v>355</v>
+        <v>328</v>
       </c>
       <c r="C30" t="s">
-        <v>354</v>
+        <v>327</v>
       </c>
       <c r="D30" t="s">
-        <v>399</v>
+        <v>380</v>
       </c>
       <c r="E30" t="s">
         <v>277</v>
@@ -15396,16 +15432,16 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>421</v>
+        <v>427</v>
       </c>
       <c r="B31" t="s">
-        <v>357</v>
+        <v>307</v>
       </c>
       <c r="C31" t="s">
-        <v>356</v>
+        <v>306</v>
       </c>
       <c r="D31" t="s">
-        <v>397</v>
+        <v>371</v>
       </c>
       <c r="E31" t="s">
         <v>277</v>
@@ -15413,104 +15449,104 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>390</v>
+        <v>425</v>
       </c>
       <c r="B32" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="C32" t="s">
-        <v>358</v>
+        <v>343</v>
       </c>
       <c r="D32" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="E32" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>409</v>
+        <v>426</v>
       </c>
       <c r="B33" t="s">
-        <v>361</v>
+        <v>323</v>
       </c>
       <c r="C33" t="s">
-        <v>360</v>
+        <v>322</v>
       </c>
       <c r="D33" t="s">
-        <v>398</v>
+        <v>378</v>
       </c>
       <c r="E33" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="B34" t="s">
-        <v>363</v>
+        <v>294</v>
       </c>
       <c r="C34" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="D34" t="s">
-        <v>400</v>
+        <v>25</v>
       </c>
       <c r="E34" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>411</v>
+        <v>429</v>
       </c>
       <c r="B35" t="s">
-        <v>365</v>
+        <v>346</v>
       </c>
       <c r="C35" t="s">
-        <v>364</v>
+        <v>345</v>
       </c>
       <c r="D35" t="s">
-        <v>401</v>
+        <v>22</v>
       </c>
       <c r="E35" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>405</v>
+        <v>324</v>
       </c>
       <c r="B36" t="s">
-        <v>367</v>
+        <v>325</v>
       </c>
       <c r="C36" t="s">
-        <v>366</v>
+        <v>326</v>
       </c>
       <c r="D36" t="s">
-        <v>402</v>
+        <v>379</v>
       </c>
       <c r="E36" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>412</v>
+        <v>428</v>
       </c>
       <c r="B37" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="C37" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="D37" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="E37" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -15523,7 +15559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9284AFDF-38E2-6C44-96DE-41340047FC8F}">
   <dimension ref="A1:C71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -16381,10 +16417,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E80B504A-1FA4-7246-8FE4-C307A80553BD}">
-  <dimension ref="A1:C1137"/>
+  <dimension ref="A1:C1140"/>
   <sheetViews>
-    <sheetView topLeftCell="A1106" zoomScale="208" zoomScaleNormal="208" workbookViewId="0">
-      <selection activeCell="C1115" sqref="C1115"/>
+    <sheetView tabSelected="1" topLeftCell="A1131" zoomScale="208" zoomScaleNormal="208" workbookViewId="0">
+      <selection activeCell="A1139" sqref="A1139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -28902,6 +28938,39 @@
         <v>3965</v>
       </c>
     </row>
+    <row r="1138" spans="1:3">
+      <c r="A1138" s="4" t="s">
+        <v>4011</v>
+      </c>
+      <c r="B1138" s="4" t="s">
+        <v>4010</v>
+      </c>
+      <c r="C1138" s="4" t="s">
+        <v>4009</v>
+      </c>
+    </row>
+    <row r="1139" spans="1:3">
+      <c r="A1139" s="4" t="s">
+        <v>4017</v>
+      </c>
+      <c r="B1139" s="4" t="s">
+        <v>4013</v>
+      </c>
+      <c r="C1139" s="4" t="s">
+        <v>4015</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:3">
+      <c r="A1140" s="4" t="s">
+        <v>4012</v>
+      </c>
+      <c r="B1140" s="4" t="s">
+        <v>4014</v>
+      </c>
+      <c r="C1140" s="4" t="s">
+        <v>4016</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add components:check_update, update new component translations, fixed datatype of blueprint.eva and blueprint.crit, update sort_by feature and blueprint import task to ensure equip attributes sorted correctly
</commit_message>
<xml_diff>
--- a/lib/assets/data_sheets/data_collected.xlsx
+++ b/lib/assets/data_sheets/data_collected.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhimoye/environment/note_titans/lib/assets/data_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D0DD6F-8D44-AA4C-957F-89D390C66EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AEFFFA1-0AD2-404E-8B4E-B2683BCBDC30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="740" windowWidth="14660" windowHeight="17080" firstSheet="4" activeTab="8" xr2:uid="{12806AD4-EDD1-E74D-A0E6-8A783616F34F}"/>
+    <workbookView xWindow="1300" yWindow="740" windowWidth="25820" windowHeight="17080" activeTab="2" xr2:uid="{12806AD4-EDD1-E74D-A0E6-8A783616F34F}"/>
   </bookViews>
   <sheets>
     <sheet name="FlashQuests" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4184" uniqueCount="4018">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4190" uniqueCount="4024">
   <si>
     <t>unlock_merchant_level</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -12739,6 +12739,30 @@
   </si>
   <si>
     <t>Gold Medal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chunk of Boots</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rusted Cannon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>靴子碎块</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>朽败大炮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rustyboots</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rustygun</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -14028,10 +14052,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C403D5DA-C305-0848-9697-99072F7D8897}">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -14653,6 +14677,28 @@
       </c>
       <c r="E52">
         <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="3" t="s">
+        <v>4018</v>
+      </c>
+      <c r="B53" t="s">
+        <v>4020</v>
+      </c>
+      <c r="C53" t="s">
+        <v>4022</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="3" t="s">
+        <v>4019</v>
+      </c>
+      <c r="B54" t="s">
+        <v>4021</v>
+      </c>
+      <c r="C54" t="s">
+        <v>4023</v>
       </c>
     </row>
   </sheetData>
@@ -16419,7 +16465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E80B504A-1FA4-7246-8FE4-C307A80553BD}">
   <dimension ref="A1:C1140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1131" zoomScale="208" zoomScaleNormal="208" workbookViewId="0">
+    <sheetView topLeftCell="A1131" zoomScale="208" zoomScaleNormal="208" workbookViewId="0">
       <selection activeCell="A1139" sqref="A1139"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
content updated to 2025/5/8, calendar replaced by the temp page
</commit_message>
<xml_diff>
--- a/lib/assets/data_sheets/data_collected.xlsx
+++ b/lib/assets/data_sheets/data_collected.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhimoye/environment/note_titans/lib/assets/data_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B8C780-4962-B843-8A4A-1BD55E83FA3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F5600E-8CBE-744E-9AFF-F8768AF29C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="740" windowWidth="16040" windowHeight="17040" activeTab="8" xr2:uid="{12806AD4-EDD1-E74D-A0E6-8A783616F34F}"/>
+    <workbookView xWindow="12860" yWindow="740" windowWidth="16040" windowHeight="17000" firstSheet="2" activeTab="8" xr2:uid="{12806AD4-EDD1-E74D-A0E6-8A783616F34F}"/>
   </bookViews>
   <sheets>
     <sheet name="FlashQuests" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4441" uniqueCount="4271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4741" uniqueCount="4569">
   <si>
     <t>unlock_merchant_level</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -13749,6 +13749,1189 @@
   </si>
   <si>
     <t>platinumelement</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Platinum Wand</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Blaze of Glory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fimbulwinter Plate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fimbulwinter Dome</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Starlight Fingers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fimbulwinter Boots</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Santa's Present Bag</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Star of the Show</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>白金魔杖</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>荣光烈焰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>漫长寒冬护甲</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>漫长寒冬头盔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>星光手套</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>漫长寒冬靴子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>圣诞老人的礼物袋</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>舞场明星</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>platinumwand</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>winterplate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>winterhelm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>newyearspear2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>newyeargloves</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>winterboots</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>christmasquiver</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>newyearamulet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Twin Fangs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>双生尖牙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lunarsword2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Copper Bite</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>铁齿铜牙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lunaraxe2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fangtian Huaji</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>方天画戟</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lunarspear2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Snake Counselor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>狡蛇顾问</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lunarmagehat2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Serpent Vestment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大蛇法袍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lunarmediumarmor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Betrayer's Hands</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>背叛者之手</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lunargloves2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ancestor Spirit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>祖先精魂</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>platinumspirit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Heart Thumper</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>怦然心动</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Backfire Hammer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Platinum Pair</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>白金双持</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sumptuous Roses</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>奢华玫瑰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lone Flowerpot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>孤独盆栽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Grandma's Teapot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>奶奶的茶壶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Squirrel Spirit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>松鼠精魂</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tournedos Rossini</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>罗西尼牛排</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>逆火锤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>artifactmace</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>valentinemace</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>valentineherb2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>valentinemeal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>squirrel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cozypotion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>platinumdualwield</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cozyherb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Year of the Snake Content Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lny2025</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LNY 2025</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蛇年内容令状</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>里路的秘密帽子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>里路的鞋子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>里路的星陨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>波利克斯的凝视</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lilumagehat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>liluwand2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lilushoes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>liluscroll</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lilu's Secret Hat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lilu's Shoes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lilu's Starfall</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pollux Focus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bjornbow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bjorn's Bow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>比约恩的弓箭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>亚米的手套</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阿尔贡之盾</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阿尔贡之盔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>泰坦护手</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>白金大酒杯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多诺万的斗篷</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阿尔贡之铠</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shoprgauntlets</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>paladinhelm2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>donovancloak</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>paladinshield</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yamigloves</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>paladinheavyarmor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>platinumpotion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Platinum Tankard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Argon's Armor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Argon's Helm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Titan Gauntlets</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yami's Gloves</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Argon's Shield</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Donovan's Cloak</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Siren's Song</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>塞壬之歌</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t15sword</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jurassicsword</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>魅魔殉道者</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Succubus Martyr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tenoch Tyrant</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>特诺克暴君</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t15axe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>metaldagger</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Electrifying Microphone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电音麦克风</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>幽灵收割者</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ghost Reaver</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t15dagger</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The Coconaught</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>椰心勃勃杖</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t15mace</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jurassicmace</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>椰心灼灼杖</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hot Coconaught</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Scream Amplifier</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>盛放利刃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t15spear</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>尖叫放大器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>metalspear</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Blossomblade</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sacrilege</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>亵渎之弓</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t15bow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>玫瑰杖</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t15wand</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>七伤笔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>paintstaff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t15staff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>奥术风向标</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Arcane Vane</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The Pain Brush</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>La Rose</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>神圣终结者</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t15gun</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t15crossbow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第七奇迹</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Seventh Wonder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Divine Eliminator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>温迪戈无人机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>双颈摇滚吉他</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rockin' Doubleneck</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>metalinstrument</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t15instrument</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t15dualwield</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>家具城</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一分为二的命运</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Twig of Two Fates</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t15herb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t15potion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jurassicpotion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Primal Fire</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ancient Waters</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>古代水域</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蛮荒火焰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>穆达拉的法令</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>部落涂鸦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tribal Scribbles</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mundra's Decree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t15scroll</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>调色板</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>paintshield</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>炽天使之凝视</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t15shield</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Seraphim Gaze</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Painted Palette</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>血石爪</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多彩戒指</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ring of Many Colors</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bloodstone Claw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t15ring</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>paintring</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trophy of Fangs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>荣誉獠牙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t15amulet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lord of the Wildwoods</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t15cloak</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>林地之主</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>trex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>platinumgolem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>白金魔像</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Platinum Golem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>霸王龙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Aura of Transmutation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>变形术气场</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Aura of Inspiration</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>灵感气场</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>paintaura</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t15aura</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rex Backpack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>霸王龙背包</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t15quiver</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dino Nuggies</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>恐龙鸡块</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t15meal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chocodragon Summit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>龙盘糕峰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t15dessert</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Teddy Bear Body</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>泰迪熊身体</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Behemoth Armor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>比蒙护甲</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t15heavyarmor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plushieheavyarmor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t15mediumarmor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蛹丝衣</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chrysalid Silks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deepsea Mageskin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Earthen Membrane</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地衣之膜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>深海法袍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t15robe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jurassicrobe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plushiehelm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>泰迪熊头</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Behemoth Skull</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Teddy Bear Head</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>比蒙头颅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t15helm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蛹面具</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>智天使斗篷</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chrysalid Mask</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cherubim Visage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t15roguehat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jurassicroguehat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t15magehat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>深海斗笠</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deepsea Kasa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>比蒙爪</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Behemoth Claws</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Teddy Bear Paws</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>泰迪熊爪爪</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plushiegauntlets</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t15gauntlets</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chrysalid Gloves</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蛹手套</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t15gloves</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Behemoth Feet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>比蒙足</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t15boots</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Teddy Bear Feet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>泰迪熊脚脚</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plushieboots</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Steel-Studded Boots</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>钢钉靴子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>飞毛腿旅人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蛹靴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chrysalid Boots</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fleetfoot Travelers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>metalshoes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t15shoes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jurassicshoes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mysterious Fossil</t>
+  </si>
+  <si>
+    <t>Dinosaur Leather</t>
+  </si>
+  <si>
+    <t>Ancient Amber</t>
+  </si>
+  <si>
+    <t>Elder Wood</t>
+  </si>
+  <si>
+    <t>Man-goroots</t>
+  </si>
+  <si>
+    <t>Full Moon Crystal</t>
+  </si>
+  <si>
+    <t>Star Metal Ingot</t>
+  </si>
+  <si>
+    <t>Kingtoplasm</t>
+  </si>
+  <si>
+    <t>Marble Pillar</t>
+  </si>
+  <si>
+    <t>神秘化石</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>恐龙皮革</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>远古琥珀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>人陀罗</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>星铁锭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>满月水晶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大理石柱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>古木</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>王质体</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>amber</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dinoleather</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>oldfossil</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tw_ancientmarble</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tw_ectoplasm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tw_elvenwood</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tw_livingroots</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tw_mooncrystal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tw_starmetal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wendigo Drone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nook &amp; Cranny</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mundrascroll</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -15102,10 +16285,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA03D614-9D25-014E-BEA0-F56DD3E0919C}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -15438,6 +16621,26 @@
         <v>45655</v>
       </c>
     </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>4341</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4342</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4340</v>
+      </c>
+      <c r="D17" t="s">
+        <v>4343</v>
+      </c>
+      <c r="E17" s="1">
+        <v>45678</v>
+      </c>
+      <c r="F17" s="1">
+        <v>45706</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15446,10 +16649,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C403D5DA-C305-0848-9697-99072F7D8897}">
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+    <sheetView topLeftCell="A40" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -16093,6 +17296,105 @@
       </c>
       <c r="C54" t="s">
         <v>4008</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>4539</v>
+      </c>
+      <c r="B55" t="s">
+        <v>4548</v>
+      </c>
+      <c r="C55" t="s">
+        <v>4559</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>4540</v>
+      </c>
+      <c r="B56" t="s">
+        <v>4549</v>
+      </c>
+      <c r="C56" t="s">
+        <v>4558</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>4541</v>
+      </c>
+      <c r="B57" t="s">
+        <v>4550</v>
+      </c>
+      <c r="C57" t="s">
+        <v>4557</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>4542</v>
+      </c>
+      <c r="B58" t="s">
+        <v>4555</v>
+      </c>
+      <c r="C58" t="s">
+        <v>4562</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>4543</v>
+      </c>
+      <c r="B59" t="s">
+        <v>4551</v>
+      </c>
+      <c r="C59" t="s">
+        <v>4563</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>4544</v>
+      </c>
+      <c r="B60" t="s">
+        <v>4553</v>
+      </c>
+      <c r="C60" t="s">
+        <v>4564</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>4545</v>
+      </c>
+      <c r="B61" t="s">
+        <v>4552</v>
+      </c>
+      <c r="C61" t="s">
+        <v>4565</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>4546</v>
+      </c>
+      <c r="B62" t="s">
+        <v>4556</v>
+      </c>
+      <c r="C62" t="s">
+        <v>4561</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>4547</v>
+      </c>
+      <c r="B63" t="s">
+        <v>4554</v>
+      </c>
+      <c r="C63" t="s">
+        <v>4560</v>
       </c>
     </row>
   </sheetData>
@@ -16351,7 +17653,7 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView topLeftCell="A15" zoomScale="112" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -17031,10 +18333,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9284AFDF-38E2-6C44-96DE-41340047FC8F}">
-  <dimension ref="A1:C71"/>
+  <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A56" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -17608,6 +18910,14 @@
         <v>3972</v>
       </c>
     </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="4" t="s">
+        <v>4327</v>
+      </c>
+      <c r="B72" t="s">
+        <v>4336</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17616,10 +18926,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E80B504A-1FA4-7246-8FE4-C307A80553BD}">
-  <dimension ref="A1:C1209"/>
+  <dimension ref="A1:C1298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1197" zoomScale="208" zoomScaleNormal="208" workbookViewId="0">
-      <selection activeCell="C1210" sqref="C1210"/>
+    <sheetView tabSelected="1" topLeftCell="A1254" zoomScale="208" zoomScaleNormal="208" workbookViewId="0">
+      <selection activeCell="C1267" sqref="C1267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -30929,6 +32239,985 @@
         <v>4270</v>
       </c>
     </row>
+    <row r="1210" spans="1:3">
+      <c r="A1210" s="4" t="s">
+        <v>4271</v>
+      </c>
+      <c r="B1210" s="4" t="s">
+        <v>4279</v>
+      </c>
+      <c r="C1210" s="4" t="s">
+        <v>4287</v>
+      </c>
+    </row>
+    <row r="1211" spans="1:3">
+      <c r="A1211" s="4" t="s">
+        <v>4272</v>
+      </c>
+      <c r="B1211" s="4" t="s">
+        <v>4280</v>
+      </c>
+      <c r="C1211" s="4" t="s">
+        <v>4290</v>
+      </c>
+    </row>
+    <row r="1212" spans="1:3">
+      <c r="A1212" s="4" t="s">
+        <v>4273</v>
+      </c>
+      <c r="B1212" s="4" t="s">
+        <v>4281</v>
+      </c>
+      <c r="C1212" s="4" t="s">
+        <v>4288</v>
+      </c>
+    </row>
+    <row r="1213" spans="1:3">
+      <c r="A1213" s="4" t="s">
+        <v>4274</v>
+      </c>
+      <c r="B1213" s="4" t="s">
+        <v>4282</v>
+      </c>
+      <c r="C1213" s="4" t="s">
+        <v>4289</v>
+      </c>
+    </row>
+    <row r="1214" spans="1:3">
+      <c r="A1214" s="4" t="s">
+        <v>4275</v>
+      </c>
+      <c r="B1214" s="4" t="s">
+        <v>4283</v>
+      </c>
+      <c r="C1214" s="4" t="s">
+        <v>4291</v>
+      </c>
+    </row>
+    <row r="1215" spans="1:3">
+      <c r="A1215" s="4" t="s">
+        <v>4276</v>
+      </c>
+      <c r="B1215" s="4" t="s">
+        <v>4284</v>
+      </c>
+      <c r="C1215" s="4" t="s">
+        <v>4292</v>
+      </c>
+    </row>
+    <row r="1216" spans="1:3">
+      <c r="A1216" s="4" t="s">
+        <v>4277</v>
+      </c>
+      <c r="B1216" s="4" t="s">
+        <v>4285</v>
+      </c>
+      <c r="C1216" s="4" t="s">
+        <v>4293</v>
+      </c>
+    </row>
+    <row r="1217" spans="1:3">
+      <c r="A1217" s="4" t="s">
+        <v>4278</v>
+      </c>
+      <c r="B1217" s="4" t="s">
+        <v>4286</v>
+      </c>
+      <c r="C1217" s="4" t="s">
+        <v>4294</v>
+      </c>
+    </row>
+    <row r="1218" spans="1:3">
+      <c r="A1218" s="4" t="s">
+        <v>4295</v>
+      </c>
+      <c r="B1218" s="4" t="s">
+        <v>4296</v>
+      </c>
+      <c r="C1218" s="4" t="s">
+        <v>4297</v>
+      </c>
+    </row>
+    <row r="1219" spans="1:3">
+      <c r="A1219" s="4" t="s">
+        <v>4298</v>
+      </c>
+      <c r="B1219" s="4" t="s">
+        <v>4299</v>
+      </c>
+      <c r="C1219" s="4" t="s">
+        <v>4300</v>
+      </c>
+    </row>
+    <row r="1220" spans="1:3">
+      <c r="A1220" s="4" t="s">
+        <v>4301</v>
+      </c>
+      <c r="B1220" s="4" t="s">
+        <v>4302</v>
+      </c>
+      <c r="C1220" s="4" t="s">
+        <v>4303</v>
+      </c>
+    </row>
+    <row r="1221" spans="1:3">
+      <c r="A1221" s="4" t="s">
+        <v>4304</v>
+      </c>
+      <c r="B1221" s="4" t="s">
+        <v>4305</v>
+      </c>
+      <c r="C1221" s="4" t="s">
+        <v>4306</v>
+      </c>
+    </row>
+    <row r="1222" spans="1:3">
+      <c r="A1222" s="4" t="s">
+        <v>4307</v>
+      </c>
+      <c r="B1222" s="4" t="s">
+        <v>4308</v>
+      </c>
+      <c r="C1222" s="4" t="s">
+        <v>4309</v>
+      </c>
+    </row>
+    <row r="1223" spans="1:3">
+      <c r="A1223" s="4" t="s">
+        <v>4310</v>
+      </c>
+      <c r="B1223" s="4" t="s">
+        <v>4311</v>
+      </c>
+      <c r="C1223" s="4" t="s">
+        <v>4312</v>
+      </c>
+    </row>
+    <row r="1224" spans="1:3">
+      <c r="A1224" s="4" t="s">
+        <v>4313</v>
+      </c>
+      <c r="B1224" s="4" t="s">
+        <v>4314</v>
+      </c>
+      <c r="C1224" s="4" t="s">
+        <v>4315</v>
+      </c>
+    </row>
+    <row r="1225" spans="1:3">
+      <c r="A1225" s="4" t="s">
+        <v>4316</v>
+      </c>
+      <c r="B1225" s="4" t="s">
+        <v>4317</v>
+      </c>
+      <c r="C1225" s="4" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="1226" spans="1:3">
+      <c r="A1226" s="4" t="s">
+        <v>4318</v>
+      </c>
+      <c r="B1226" s="4" t="s">
+        <v>4331</v>
+      </c>
+      <c r="C1226" s="4" t="s">
+        <v>4332</v>
+      </c>
+    </row>
+    <row r="1227" spans="1:3">
+      <c r="A1227" s="4" t="s">
+        <v>4319</v>
+      </c>
+      <c r="B1227" s="4" t="s">
+        <v>4320</v>
+      </c>
+      <c r="C1227" s="4" t="s">
+        <v>4338</v>
+      </c>
+    </row>
+    <row r="1228" spans="1:3">
+      <c r="A1228" s="4" t="s">
+        <v>4321</v>
+      </c>
+      <c r="B1228" s="4" t="s">
+        <v>4322</v>
+      </c>
+      <c r="C1228" s="4" t="s">
+        <v>4334</v>
+      </c>
+    </row>
+    <row r="1229" spans="1:3">
+      <c r="A1229" s="4" t="s">
+        <v>4323</v>
+      </c>
+      <c r="B1229" s="4" t="s">
+        <v>4324</v>
+      </c>
+      <c r="C1229" s="4" t="s">
+        <v>4339</v>
+      </c>
+    </row>
+    <row r="1230" spans="1:3">
+      <c r="A1230" s="4" t="s">
+        <v>4325</v>
+      </c>
+      <c r="B1230" s="4" t="s">
+        <v>4326</v>
+      </c>
+      <c r="C1230" s="4" t="s">
+        <v>4337</v>
+      </c>
+    </row>
+    <row r="1231" spans="1:3">
+      <c r="A1231" s="4" t="s">
+        <v>4329</v>
+      </c>
+      <c r="B1231" s="4" t="s">
+        <v>4330</v>
+      </c>
+      <c r="C1231" s="4" t="s">
+        <v>4335</v>
+      </c>
+    </row>
+    <row r="1232" spans="1:3">
+      <c r="A1232" s="4" t="s">
+        <v>4327</v>
+      </c>
+      <c r="B1232" s="4" t="s">
+        <v>4328</v>
+      </c>
+      <c r="C1232" s="4" t="s">
+        <v>4336</v>
+      </c>
+    </row>
+    <row r="1233" spans="1:3">
+      <c r="A1233" s="4" t="s">
+        <v>4352</v>
+      </c>
+      <c r="B1233" s="4" t="s">
+        <v>4344</v>
+      </c>
+      <c r="C1233" s="4" t="s">
+        <v>4348</v>
+      </c>
+    </row>
+    <row r="1234" spans="1:3">
+      <c r="A1234" s="4" t="s">
+        <v>4353</v>
+      </c>
+      <c r="B1234" s="4" t="s">
+        <v>4345</v>
+      </c>
+      <c r="C1234" s="4" t="s">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="1235" spans="1:3">
+      <c r="A1235" s="4" t="s">
+        <v>4354</v>
+      </c>
+      <c r="B1235" s="4" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C1235" s="4" t="s">
+        <v>4351</v>
+      </c>
+    </row>
+    <row r="1236" spans="1:3">
+      <c r="A1236" s="4" t="s">
+        <v>4355</v>
+      </c>
+      <c r="B1236" s="4" t="s">
+        <v>4347</v>
+      </c>
+      <c r="C1236" s="4" t="s">
+        <v>4349</v>
+      </c>
+    </row>
+    <row r="1237" spans="1:3">
+      <c r="A1237" s="4" t="s">
+        <v>4357</v>
+      </c>
+      <c r="B1237" s="4" t="s">
+        <v>4358</v>
+      </c>
+      <c r="C1237" s="4" t="s">
+        <v>4356</v>
+      </c>
+    </row>
+    <row r="1238" spans="1:3">
+      <c r="A1238" s="4" t="s">
+        <v>4373</v>
+      </c>
+      <c r="B1238" s="4" t="s">
+        <v>4363</v>
+      </c>
+      <c r="C1238" s="4" t="s">
+        <v>4372</v>
+      </c>
+    </row>
+    <row r="1239" spans="1:3">
+      <c r="A1239" s="4" t="s">
+        <v>4374</v>
+      </c>
+      <c r="B1239" s="4" t="s">
+        <v>4365</v>
+      </c>
+      <c r="C1239" s="4" t="s">
+        <v>4371</v>
+      </c>
+    </row>
+    <row r="1240" spans="1:3">
+      <c r="A1240" s="4" t="s">
+        <v>4375</v>
+      </c>
+      <c r="B1240" s="4" t="s">
+        <v>4361</v>
+      </c>
+      <c r="C1240" s="4" t="s">
+        <v>4367</v>
+      </c>
+    </row>
+    <row r="1241" spans="1:3">
+      <c r="A1241" s="4" t="s">
+        <v>4376</v>
+      </c>
+      <c r="B1241" s="4" t="s">
+        <v>4362</v>
+      </c>
+      <c r="C1241" s="4" t="s">
+        <v>4366</v>
+      </c>
+    </row>
+    <row r="1242" spans="1:3">
+      <c r="A1242" s="4" t="s">
+        <v>4377</v>
+      </c>
+      <c r="B1242" s="4" t="s">
+        <v>4359</v>
+      </c>
+      <c r="C1242" s="4" t="s">
+        <v>4370</v>
+      </c>
+    </row>
+    <row r="1243" spans="1:3">
+      <c r="A1243" s="4" t="s">
+        <v>4378</v>
+      </c>
+      <c r="B1243" s="4" t="s">
+        <v>4360</v>
+      </c>
+      <c r="C1243" s="4" t="s">
+        <v>4369</v>
+      </c>
+    </row>
+    <row r="1244" spans="1:3">
+      <c r="A1244" s="4" t="s">
+        <v>4379</v>
+      </c>
+      <c r="B1244" s="4" t="s">
+        <v>4364</v>
+      </c>
+      <c r="C1244" s="4" t="s">
+        <v>4368</v>
+      </c>
+    </row>
+    <row r="1245" spans="1:3">
+      <c r="A1245" s="4" t="s">
+        <v>4380</v>
+      </c>
+      <c r="B1245" s="4" t="s">
+        <v>4381</v>
+      </c>
+      <c r="C1245" s="4" t="s">
+        <v>4382</v>
+      </c>
+    </row>
+    <row r="1246" spans="1:3">
+      <c r="A1246" s="4" t="s">
+        <v>4385</v>
+      </c>
+      <c r="B1246" s="4" t="s">
+        <v>4384</v>
+      </c>
+      <c r="C1246" s="4" t="s">
+        <v>4383</v>
+      </c>
+    </row>
+    <row r="1247" spans="1:3">
+      <c r="A1247" s="4" t="s">
+        <v>4386</v>
+      </c>
+      <c r="B1247" s="4" t="s">
+        <v>4387</v>
+      </c>
+      <c r="C1247" s="4" t="s">
+        <v>4388</v>
+      </c>
+    </row>
+    <row r="1248" spans="1:3">
+      <c r="A1248" s="4" t="s">
+        <v>4390</v>
+      </c>
+      <c r="B1248" s="4" t="s">
+        <v>4391</v>
+      </c>
+      <c r="C1248" s="4" t="s">
+        <v>4389</v>
+      </c>
+    </row>
+    <row r="1249" spans="1:3">
+      <c r="A1249" s="4" t="s">
+        <v>4393</v>
+      </c>
+      <c r="B1249" s="4" t="s">
+        <v>4392</v>
+      </c>
+      <c r="C1249" s="4" t="s">
+        <v>4394</v>
+      </c>
+    </row>
+    <row r="1250" spans="1:3">
+      <c r="A1250" s="4" t="s">
+        <v>4395</v>
+      </c>
+      <c r="B1250" s="4" t="s">
+        <v>4396</v>
+      </c>
+      <c r="C1250" s="4" t="s">
+        <v>4397</v>
+      </c>
+    </row>
+    <row r="1251" spans="1:3">
+      <c r="A1251" s="4" t="s">
+        <v>4400</v>
+      </c>
+      <c r="B1251" s="4" t="s">
+        <v>4399</v>
+      </c>
+      <c r="C1251" s="4" t="s">
+        <v>4398</v>
+      </c>
+    </row>
+    <row r="1252" spans="1:3">
+      <c r="A1252" s="4" t="s">
+        <v>4401</v>
+      </c>
+      <c r="B1252" s="4" t="s">
+        <v>4404</v>
+      </c>
+      <c r="C1252" s="4" t="s">
+        <v>4405</v>
+      </c>
+    </row>
+    <row r="1253" spans="1:3">
+      <c r="A1253" s="4" t="s">
+        <v>4406</v>
+      </c>
+      <c r="B1253" s="4" t="s">
+        <v>4402</v>
+      </c>
+      <c r="C1253" s="4" t="s">
+        <v>4403</v>
+      </c>
+    </row>
+    <row r="1254" spans="1:3">
+      <c r="A1254" s="4" t="s">
+        <v>4407</v>
+      </c>
+      <c r="B1254" s="4" t="s">
+        <v>4408</v>
+      </c>
+      <c r="C1254" s="4" t="s">
+        <v>4409</v>
+      </c>
+    </row>
+    <row r="1255" spans="1:3">
+      <c r="A1255" s="4" t="s">
+        <v>4416</v>
+      </c>
+      <c r="B1255" s="4" t="s">
+        <v>4415</v>
+      </c>
+      <c r="C1255" s="4" t="s">
+        <v>4414</v>
+      </c>
+    </row>
+    <row r="1256" spans="1:3">
+      <c r="A1256" s="4" t="s">
+        <v>4417</v>
+      </c>
+      <c r="B1256" s="4" t="s">
+        <v>4412</v>
+      </c>
+      <c r="C1256" s="4" t="s">
+        <v>4413</v>
+      </c>
+    </row>
+    <row r="1257" spans="1:3">
+      <c r="A1257" s="4" t="s">
+        <v>4418</v>
+      </c>
+      <c r="B1257" s="4" t="s">
+        <v>4410</v>
+      </c>
+      <c r="C1257" s="4" t="s">
+        <v>4411</v>
+      </c>
+    </row>
+    <row r="1258" spans="1:3">
+      <c r="A1258" s="4" t="s">
+        <v>4423</v>
+      </c>
+      <c r="B1258" s="4" t="s">
+        <v>4422</v>
+      </c>
+      <c r="C1258" s="4" t="s">
+        <v>4421</v>
+      </c>
+    </row>
+    <row r="1259" spans="1:3">
+      <c r="A1259" s="4" t="s">
+        <v>4424</v>
+      </c>
+      <c r="B1259" s="4" t="s">
+        <v>4419</v>
+      </c>
+      <c r="C1259" s="4" t="s">
+        <v>4420</v>
+      </c>
+    </row>
+    <row r="1260" spans="1:3">
+      <c r="A1260" s="4" t="s">
+        <v>4427</v>
+      </c>
+      <c r="B1260" s="4" t="s">
+        <v>4426</v>
+      </c>
+      <c r="C1260" s="4" t="s">
+        <v>4428</v>
+      </c>
+    </row>
+    <row r="1261" spans="1:3">
+      <c r="A1261" s="4" t="s">
+        <v>4566</v>
+      </c>
+      <c r="B1261" s="4" t="s">
+        <v>4425</v>
+      </c>
+      <c r="C1261" s="4" t="s">
+        <v>4429</v>
+      </c>
+    </row>
+    <row r="1262" spans="1:3">
+      <c r="A1262" s="4" t="s">
+        <v>4567</v>
+      </c>
+      <c r="B1262" s="4" t="s">
+        <v>4431</v>
+      </c>
+      <c r="C1262" s="4" t="s">
+        <v>4430</v>
+      </c>
+    </row>
+    <row r="1263" spans="1:3">
+      <c r="A1263" s="4" t="s">
+        <v>4433</v>
+      </c>
+      <c r="B1263" s="4" t="s">
+        <v>4432</v>
+      </c>
+      <c r="C1263" s="4" t="s">
+        <v>4434</v>
+      </c>
+    </row>
+    <row r="1264" spans="1:3">
+      <c r="A1264" s="4" t="s">
+        <v>4437</v>
+      </c>
+      <c r="B1264" s="4" t="s">
+        <v>4440</v>
+      </c>
+      <c r="C1264" s="4" t="s">
+        <v>4435</v>
+      </c>
+    </row>
+    <row r="1265" spans="1:3">
+      <c r="A1265" s="4" t="s">
+        <v>4438</v>
+      </c>
+      <c r="B1265" s="4" t="s">
+        <v>4439</v>
+      </c>
+      <c r="C1265" s="4" t="s">
+        <v>4436</v>
+      </c>
+    </row>
+    <row r="1266" spans="1:3">
+      <c r="A1266" s="4" t="s">
+        <v>4443</v>
+      </c>
+      <c r="B1266" s="4" t="s">
+        <v>4442</v>
+      </c>
+      <c r="C1266" s="4" t="s">
+        <v>4445</v>
+      </c>
+    </row>
+    <row r="1267" spans="1:3">
+      <c r="A1267" s="4" t="s">
+        <v>4444</v>
+      </c>
+      <c r="B1267" s="4" t="s">
+        <v>4441</v>
+      </c>
+      <c r="C1267" s="4" t="s">
+        <v>4568</v>
+      </c>
+    </row>
+    <row r="1268" spans="1:3">
+      <c r="A1268" s="4" t="s">
+        <v>4485</v>
+      </c>
+      <c r="B1268" s="4" t="s">
+        <v>4486</v>
+      </c>
+      <c r="C1268" s="4" t="s">
+        <v>4490</v>
+      </c>
+    </row>
+    <row r="1269" spans="1:3">
+      <c r="A1269" s="4" t="s">
+        <v>4487</v>
+      </c>
+      <c r="B1269" s="4" t="s">
+        <v>4488</v>
+      </c>
+      <c r="C1269" s="4" t="s">
+        <v>4489</v>
+      </c>
+    </row>
+    <row r="1270" spans="1:3">
+      <c r="A1270" s="4" t="s">
+        <v>4493</v>
+      </c>
+      <c r="B1270" s="4" t="s">
+        <v>4492</v>
+      </c>
+      <c r="C1270" s="4" t="s">
+        <v>4491</v>
+      </c>
+    </row>
+    <row r="1271" spans="1:3">
+      <c r="A1271" s="4" t="s">
+        <v>4494</v>
+      </c>
+      <c r="B1271" s="4" t="s">
+        <v>4497</v>
+      </c>
+      <c r="C1271" s="4" t="s">
+        <v>4498</v>
+      </c>
+    </row>
+    <row r="1272" spans="1:3">
+      <c r="A1272" s="4" t="s">
+        <v>4495</v>
+      </c>
+      <c r="B1272" s="4" t="s">
+        <v>4496</v>
+      </c>
+      <c r="C1272" s="4" t="s">
+        <v>4499</v>
+      </c>
+    </row>
+    <row r="1273" spans="1:3">
+      <c r="A1273" s="4" t="s">
+        <v>4502</v>
+      </c>
+      <c r="B1273" s="4" t="s">
+        <v>4504</v>
+      </c>
+      <c r="C1273" s="4" t="s">
+        <v>4505</v>
+      </c>
+    </row>
+    <row r="1274" spans="1:3">
+      <c r="A1274" s="4" t="s">
+        <v>4503</v>
+      </c>
+      <c r="B1274" s="4" t="s">
+        <v>4501</v>
+      </c>
+      <c r="C1274" s="4" t="s">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="1275" spans="1:3">
+      <c r="A1275" s="4" t="s">
+        <v>4508</v>
+      </c>
+      <c r="B1275" s="4" t="s">
+        <v>4506</v>
+      </c>
+      <c r="C1275" s="4" t="s">
+        <v>4510</v>
+      </c>
+    </row>
+    <row r="1276" spans="1:3">
+      <c r="A1276" s="4" t="s">
+        <v>4509</v>
+      </c>
+      <c r="B1276" s="4" t="s">
+        <v>4507</v>
+      </c>
+      <c r="C1276" s="4" t="s">
+        <v>4511</v>
+      </c>
+    </row>
+    <row r="1277" spans="1:3">
+      <c r="A1277" s="4" t="s">
+        <v>4514</v>
+      </c>
+      <c r="B1277" s="4" t="s">
+        <v>4513</v>
+      </c>
+      <c r="C1277" s="4" t="s">
+        <v>4512</v>
+      </c>
+    </row>
+    <row r="1278" spans="1:3">
+      <c r="A1278" s="4" t="s">
+        <v>4517</v>
+      </c>
+      <c r="B1278" s="4" t="s">
+        <v>4518</v>
+      </c>
+      <c r="C1278" s="4" t="s">
+        <v>4519</v>
+      </c>
+    </row>
+    <row r="1279" spans="1:3">
+      <c r="A1279" s="4" t="s">
+        <v>4516</v>
+      </c>
+      <c r="B1279" s="4" t="s">
+        <v>4515</v>
+      </c>
+      <c r="C1279" s="4" t="s">
+        <v>4520</v>
+      </c>
+    </row>
+    <row r="1280" spans="1:3">
+      <c r="A1280" s="4" t="s">
+        <v>4521</v>
+      </c>
+      <c r="B1280" s="4" t="s">
+        <v>4522</v>
+      </c>
+      <c r="C1280" s="4" t="s">
+        <v>4523</v>
+      </c>
+    </row>
+    <row r="1281" spans="1:3">
+      <c r="A1281" s="4" t="s">
+        <v>4524</v>
+      </c>
+      <c r="B1281" s="4" t="s">
+        <v>4525</v>
+      </c>
+      <c r="C1281" s="4" t="s">
+        <v>4526</v>
+      </c>
+    </row>
+    <row r="1282" spans="1:3">
+      <c r="A1282" s="4" t="s">
+        <v>4527</v>
+      </c>
+      <c r="B1282" s="4" t="s">
+        <v>4528</v>
+      </c>
+      <c r="C1282" s="4" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="1283" spans="1:3">
+      <c r="A1283" s="4" t="s">
+        <v>4530</v>
+      </c>
+      <c r="B1283" s="4" t="s">
+        <v>4531</v>
+      </c>
+      <c r="C1283" s="4" t="s">
+        <v>4536</v>
+      </c>
+    </row>
+    <row r="1284" spans="1:3">
+      <c r="A1284" s="4" t="s">
+        <v>4534</v>
+      </c>
+      <c r="B1284" s="4" t="s">
+        <v>4533</v>
+      </c>
+      <c r="C1284" s="4" t="s">
+        <v>4537</v>
+      </c>
+    </row>
+    <row r="1285" spans="1:3">
+      <c r="A1285" s="4" t="s">
+        <v>4535</v>
+      </c>
+      <c r="B1285" s="4" t="s">
+        <v>4532</v>
+      </c>
+      <c r="C1285" s="4" t="s">
+        <v>4538</v>
+      </c>
+    </row>
+    <row r="1286" spans="1:3">
+      <c r="A1286" s="4" t="s">
+        <v>4451</v>
+      </c>
+      <c r="B1286" s="4" t="s">
+        <v>4446</v>
+      </c>
+      <c r="C1286" s="4" t="s">
+        <v>4447</v>
+      </c>
+    </row>
+    <row r="1287" spans="1:3">
+      <c r="A1287" s="4" t="s">
+        <v>4450</v>
+      </c>
+      <c r="B1287" s="4" t="s">
+        <v>4448</v>
+      </c>
+      <c r="C1287" s="4" t="s">
+        <v>4449</v>
+      </c>
+    </row>
+    <row r="1288" spans="1:3">
+      <c r="A1288" s="4" t="s">
+        <v>4476</v>
+      </c>
+      <c r="B1288" s="4" t="s">
+        <v>4477</v>
+      </c>
+      <c r="C1288" s="4" t="s">
+        <v>4478</v>
+      </c>
+    </row>
+    <row r="1289" spans="1:3">
+      <c r="A1289" s="4" t="s">
+        <v>4461</v>
+      </c>
+      <c r="B1289" s="4" t="s">
+        <v>4463</v>
+      </c>
+      <c r="C1289" s="4" t="s">
+        <v>4462</v>
+      </c>
+    </row>
+    <row r="1290" spans="1:3">
+      <c r="A1290" s="4" t="s">
+        <v>4455</v>
+      </c>
+      <c r="B1290" s="4" t="s">
+        <v>4452</v>
+      </c>
+      <c r="C1290" s="4" t="s">
+        <v>4456</v>
+      </c>
+    </row>
+    <row r="1291" spans="1:3">
+      <c r="A1291" s="4" t="s">
+        <v>4454</v>
+      </c>
+      <c r="B1291" s="4" t="s">
+        <v>4453</v>
+      </c>
+      <c r="C1291" s="4" t="s">
+        <v>4457</v>
+      </c>
+    </row>
+    <row r="1292" spans="1:3">
+      <c r="A1292" s="4" t="s">
+        <v>4458</v>
+      </c>
+      <c r="B1292" s="4" t="s">
+        <v>4459</v>
+      </c>
+      <c r="C1292" s="4" t="s">
+        <v>4460</v>
+      </c>
+    </row>
+    <row r="1293" spans="1:3">
+      <c r="A1293" s="4" t="s">
+        <v>4467</v>
+      </c>
+      <c r="B1293" s="4" t="s">
+        <v>4466</v>
+      </c>
+      <c r="C1293" s="4" t="s">
+        <v>4465</v>
+      </c>
+    </row>
+    <row r="1294" spans="1:3">
+      <c r="A1294" s="4" t="s">
+        <v>4468</v>
+      </c>
+      <c r="B1294" s="4" t="s">
+        <v>4469</v>
+      </c>
+      <c r="C1294" s="4" t="s">
+        <v>4464</v>
+      </c>
+    </row>
+    <row r="1295" spans="1:3">
+      <c r="A1295" s="4" t="s">
+        <v>4479</v>
+      </c>
+      <c r="B1295" s="4" t="s">
+        <v>4480</v>
+      </c>
+      <c r="C1295" s="4" t="s">
+        <v>4481</v>
+      </c>
+    </row>
+    <row r="1296" spans="1:3">
+      <c r="A1296" s="4" t="s">
+        <v>4482</v>
+      </c>
+      <c r="B1296" s="4" t="s">
+        <v>4483</v>
+      </c>
+      <c r="C1296" s="4" t="s">
+        <v>4484</v>
+      </c>
+    </row>
+    <row r="1297" spans="1:3">
+      <c r="A1297" s="4" t="s">
+        <v>4470</v>
+      </c>
+      <c r="B1297" s="4" t="s">
+        <v>4471</v>
+      </c>
+      <c r="C1297" s="4" t="s">
+        <v>4475</v>
+      </c>
+    </row>
+    <row r="1298" spans="1:3">
+      <c r="A1298" s="4" t="s">
+        <v>4472</v>
+      </c>
+      <c r="B1298" s="4" t="s">
+        <v>4473</v>
+      </c>
+      <c r="C1298" s="4" t="s">
+        <v>4474</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>